<commit_message>
adding another excel template
</commit_message>
<xml_diff>
--- a/public/assets/excel/ImportUsersTemplate.xlsx
+++ b/public/assets/excel/ImportUsersTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bruno/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7D5A5A3-3E50-9747-A503-CE079018C906}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9090FDE-7AE6-604A-B80F-AB8B4BB0DA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" xr2:uid="{4039FB99-F224-C344-8945-F5147FF21724}"/>
   </bookViews>
@@ -25,16 +25,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Name or Email or Username</t>
+    <r>
+      <t xml:space="preserve">Please Follow the following instruction: Add the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>username</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the user that you wish to login. Use one entry per row, as showed in the example. Use Column A. PS: Please erase the example written in this file.</t>
+    </r>
+  </si>
+  <si>
+    <t>example username</t>
+  </si>
+  <si>
+    <t>example name</t>
+  </si>
+  <si>
+    <t>example@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,9 +117,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -88,16 +177,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,23 +609,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426B51B3-D6E3-D24B-82A7-9B47D66A4CA8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" thickBottom="1"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" thickBot="1">
+      <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" thickBot="1">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" thickBot="1">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" thickBot="1">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" thickBot="1">
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{FD2A403A-FD29-EA47-9951-8163E5BD77E8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>